<commit_message>
se quita inserción cuenta nequi
</commit_message>
<xml_diff>
--- a/qam-front/src/assets/Layout_carga_usuario_CO.xlsx
+++ b/qam-front/src/assets/Layout_carga_usuario_CO.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="68">
   <si>
     <t>Primer Apellido</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Correo electrónico</t>
   </si>
   <si>
-    <t>Cuenta Nequi</t>
-  </si>
-  <si>
     <t>Genero</t>
   </si>
   <si>
@@ -81,9 +78,6 @@
     <t xml:space="preserve">Nombre </t>
   </si>
   <si>
-    <t>Fecha de nacimiento dd/mm/aa</t>
-  </si>
-  <si>
     <t>Tipo de Documento de ID</t>
   </si>
   <si>
@@ -216,9 +210,6 @@
     <t>(001) Bancolombia</t>
   </si>
   <si>
-    <t>(021) Provincial</t>
-  </si>
-  <si>
     <t>(002) Banco Caja Social BCSC</t>
   </si>
   <si>
@@ -232,6 +223,12 @@
   </si>
   <si>
     <t>NIT</t>
+  </si>
+  <si>
+    <t>Fecha de nacimiento dd/mm/aaaa</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -242,7 +239,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -305,6 +302,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -462,7 +474,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -476,24 +488,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -521,44 +521,53 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8"/>
@@ -1087,113 +1096,115 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.90625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="18.08984375" style="12" customWidth="1"/>
-    <col min="3" max="3" width="21.08984375" style="30" customWidth="1"/>
-    <col min="4" max="4" width="28.1796875" style="30" customWidth="1"/>
-    <col min="5" max="5" width="30.36328125" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.36328125" style="33" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.81640625" style="27" customWidth="1"/>
-    <col min="8" max="8" width="22.1796875" style="9" customWidth="1"/>
-    <col min="9" max="9" width="27.453125" style="9" customWidth="1"/>
-    <col min="10" max="10" width="22.08984375" style="25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.54296875" style="12" customWidth="1"/>
-    <col min="12" max="12" width="17" style="29" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.90625" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.7265625" style="7" customWidth="1"/>
-    <col min="15" max="15" width="19.7265625" style="12" customWidth="1"/>
-    <col min="16" max="16" width="29" style="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="26.90625" style="12" customWidth="1"/>
-    <col min="18" max="18" width="21.54296875" style="30" customWidth="1"/>
-    <col min="19" max="19" width="20.1796875" style="30" customWidth="1"/>
-    <col min="20" max="16384" width="10.90625" style="7"/>
+    <col min="1" max="1" width="21.90625" style="28" customWidth="1"/>
+    <col min="2" max="2" width="18.08984375" style="28" customWidth="1"/>
+    <col min="3" max="3" width="21.08984375" style="29" customWidth="1"/>
+    <col min="4" max="4" width="28.1796875" style="29" customWidth="1"/>
+    <col min="5" max="5" width="30.36328125" style="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.36328125" style="30" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.81640625" style="35" customWidth="1"/>
+    <col min="8" max="8" width="22.1796875" style="31" customWidth="1"/>
+    <col min="9" max="9" width="22.08984375" style="32" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.54296875" style="28" customWidth="1"/>
+    <col min="11" max="11" width="17" style="33" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.90625" style="34" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.7265625" style="32" customWidth="1"/>
+    <col min="14" max="14" width="19.7265625" style="28" customWidth="1"/>
+    <col min="15" max="15" width="29" style="28" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.90625" style="28" customWidth="1"/>
+    <col min="17" max="17" width="21.54296875" style="29" customWidth="1"/>
+    <col min="18" max="18" width="20.1796875" style="29" customWidth="1"/>
+    <col min="19" max="16384" width="10.90625" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="37" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="16" t="s">
+    <row r="1" spans="1:18" s="22" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="K1" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="L1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="N1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="20" t="s">
+      <c r="O1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q1" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="R1" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="S1" s="21" t="s">
+      <c r="P1" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" s="15" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="31"/>
+      <c r="R1" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="J2" s="27"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="23"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="G4" s="30"/>
     </row>
   </sheetData>
   <dataValidations count="5">
@@ -1206,11 +1217,11 @@
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Introduce un email válido" sqref="H2:H1048576">
       <formula1>ISNUMBER(SEARCH("@", H2))</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="La longitud de la cuenta no cumple con los 10 dígitos requeridos" sqref="S2:S1048576">
+    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="La longitud de la cuenta no cumple con los 10 dígitos requeridos" sqref="R2:R1048576">
       <formula1>10</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Coloque el número de teléfono con iniciando con &quot;+&quot;_x000a_" sqref="G2:G1048576">
-      <formula1>10</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G3 G5:G1048576">
+      <formula1>ISNUMBER(SEARCH("+", G2))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1228,31 +1239,31 @@
           <x14:formula1>
             <xm:f>Catalogos!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K1048576</xm:sqref>
+          <xm:sqref>J2:J1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Catalogos!$G$2:$G$34</xm:f>
           </x14:formula1>
-          <xm:sqref>P2:P1048576</xm:sqref>
+          <xm:sqref>O2:O1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Catalogos!$I$2:$I$5</xm:f>
+            <xm:f>Catalogos!$E$2:$E$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>K2:K1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Catalogos!$K$2:$K$3</xm:f>
           </x14:formula1>
           <xm:sqref>Q2:Q1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Catalogos!$E$2:$E$5</xm:f>
+            <xm:f>Catalogos!$I$2:$I$4</xm:f>
           </x14:formula1>
-          <xm:sqref>L2:L1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Catalogos!$K$2:$K$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>R2:R1048576</xm:sqref>
+          <xm:sqref>P2:P1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1266,7 +1277,7 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1283,238 +1294,237 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>27</v>
+        <v>5</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="M1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="27" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>66</v>
+        <v>14</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="M2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="27.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>67</v>
+        <v>15</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="E5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="E5" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="8" t="s">
+      <c r="I6" s="36"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G7" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G6" s="8" t="s">
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G8" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="G7" s="8" t="s">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G9" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="G8" s="8" t="s">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G10" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="G9" s="8" t="s">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G11" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="G10" s="8" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G12" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="G11" s="8" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G13" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="G12" s="8" t="s">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G14" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="G13" s="8" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G15" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="G14" s="8" t="s">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G16" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="G15" s="8" t="s">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G17" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="G16" s="8" t="s">
+    <row r="18" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G18" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G17" s="8" t="s">
+    <row r="19" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G19" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G18" s="8" t="s">
+    <row r="20" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G20" s="7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G19" s="8" t="s">
+    <row r="21" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G21" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G20" s="8" t="s">
+    <row r="22" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G22" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G21" s="8" t="s">
+    <row r="23" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G23" s="7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G22" s="8" t="s">
+    <row r="24" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G24" s="7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G23" s="8" t="s">
+    <row r="25" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G25" s="7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G24" s="8" t="s">
+    <row r="26" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G26" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G25" s="8" t="s">
+    <row r="27" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G27" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G26" s="8" t="s">
+    <row r="28" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G28" s="7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G27" s="8" t="s">
+    <row r="29" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G29" s="7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G28" s="8" t="s">
+    <row r="30" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G30" s="7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G29" s="8" t="s">
+    <row r="31" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G31" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G30" s="8" t="s">
+    <row r="32" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G32" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G31" s="8" t="s">
+    <row r="33" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G33" s="7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G32" s="8" t="s">
+    <row r="34" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G34" s="7" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G33" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="34" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G34" s="8" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>